<commit_message>
Add structural superimposition photos
</commit_message>
<xml_diff>
--- a/QTY Design/Comparison.xlsx
+++ b/QTY Design/Comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\Rhodopsins_QTY\QTY Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4334F13F-6D06-452D-B025-C9BA74E0F22E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334802A4-989A-4D3F-AD55-13E89BFF4D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="6765" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WT-QTY-EXP" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="28">
   <si>
     <t>OPN1MW</t>
   </si>
@@ -108,16 +108,22 @@
     <t>WT</t>
   </si>
   <si>
-    <t>EXP</t>
-  </si>
-  <si>
     <t>Monomer-trimer</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>BR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -201,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -219,17 +225,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -513,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D856C77-9565-4F87-ABAB-A87EC8DCE168}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -540,27 +549,41 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="B2" s="9">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="B3" s="9">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="B4" s="9">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -568,19 +591,27 @@
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="B5" s="9">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0.999</v>
+      </c>
     </row>
     <row r="6" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="B6" s="9">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -588,11 +619,13 @@
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="B7" s="9">
+        <v>0.307</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -600,11 +633,13 @@
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="B8" s="9">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -612,11 +647,13 @@
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="B9" s="9">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -624,11 +661,13 @@
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="B10" s="9">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -636,33 +675,57 @@
       <c r="A11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="B11" s="9">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0.252</v>
+      </c>
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="B12" s="9">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="B13" s="9">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0.57099999999999995</v>
+      </c>
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="B14" s="9">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0.58399999999999996</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -673,9 +736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A17" sqref="A10:XFD17"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -716,12 +777,24 @@
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="9">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="D2" s="9">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="E2" s="9">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="F2" s="9">
+        <v>1.6160000000000001</v>
+      </c>
+      <c r="G2" s="9">
+        <v>1.0089999999999999</v>
+      </c>
+      <c r="H2" s="9">
+        <v>1.2450000000000001</v>
+      </c>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
@@ -734,11 +807,21 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="D3" s="9">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="F3" s="9">
+        <v>1.897</v>
+      </c>
+      <c r="G3" s="9">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="H3" s="9">
+        <v>1.5169999999999999</v>
+      </c>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
@@ -754,10 +837,18 @@
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="E4" s="9">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="F4" s="9">
+        <v>2.351</v>
+      </c>
+      <c r="G4" s="9">
+        <v>1.101</v>
+      </c>
+      <c r="H4" s="9">
+        <v>2.2949999999999999</v>
+      </c>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
@@ -776,9 +867,15 @@
       <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="F5" s="9">
+        <v>2.2360000000000002</v>
+      </c>
+      <c r="G5" s="9">
+        <v>1.0309999999999999</v>
+      </c>
+      <c r="H5" s="9">
+        <v>1.8640000000000001</v>
+      </c>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
@@ -800,8 +897,12 @@
       <c r="F6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="G6" s="9">
+        <v>1.0109999999999999</v>
+      </c>
+      <c r="H6" s="9">
+        <v>1.155</v>
+      </c>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
@@ -826,7 +927,9 @@
       <c r="G7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="9">
+        <v>1.0109999999999999</v>
+      </c>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
@@ -892,12 +995,24 @@
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="C12" s="9">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="E12" s="9">
+        <v>1.0449999999999999</v>
+      </c>
+      <c r="F12" s="9">
+        <v>1.613</v>
+      </c>
+      <c r="G12" s="9">
+        <v>1.1519999999999999</v>
+      </c>
+      <c r="H12" s="9">
+        <v>1.3720000000000001</v>
+      </c>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
@@ -910,11 +1025,21 @@
       <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="D13" s="9">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1.052</v>
+      </c>
+      <c r="F13" s="9">
+        <v>1.6539999999999999</v>
+      </c>
+      <c r="G13" s="9">
+        <v>1.155</v>
+      </c>
+      <c r="H13" s="9">
+        <v>1.141</v>
+      </c>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
@@ -930,10 +1055,18 @@
       <c r="D14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="E14" s="9">
+        <v>1.014</v>
+      </c>
+      <c r="F14" s="9">
+        <v>2.3159999999999998</v>
+      </c>
+      <c r="G14" s="9">
+        <v>1.1060000000000001</v>
+      </c>
+      <c r="H14" s="9">
+        <v>2.073</v>
+      </c>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
@@ -952,9 +1085,15 @@
       <c r="E15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="F15" s="9">
+        <v>1.96</v>
+      </c>
+      <c r="G15" s="9">
+        <v>1.0169999999999999</v>
+      </c>
+      <c r="H15" s="9">
+        <v>2.6829999999999998</v>
+      </c>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
@@ -976,8 +1115,12 @@
       <c r="F16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="G16" s="9">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="H16" s="9">
+        <v>1.194</v>
+      </c>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
@@ -1002,7 +1145,9 @@
       <c r="G17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="2"/>
+      <c r="H17" s="9">
+        <v>1.1419999999999999</v>
+      </c>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
@@ -1039,63 +1184,74 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4911FA70-48E6-48E4-9139-2D9F96EC0E56}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="4.90625" customWidth="1"/>
+    <col min="4" max="4" width="4.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="E1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10"/>
-    </row>
-    <row r="3" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="E2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-    </row>
-    <row r="4" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
-    </row>
-    <row r="5" spans="1:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11"/>
+      <c r="E3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B4:C4"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
clean up raw structures, keeping only number 0; hydrophobicity graphs; reorganize structures directory; save loops-cut structures
</commit_message>
<xml_diff>
--- a/QTY Design/Comparison.xlsx
+++ b/QTY Design/Comparison.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\Rhodopsins_QTY\QTY Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E7FD1B-D9FA-4874-A72E-E8556545D133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09912A47-1702-4147-B522-7A2C6285364C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WT-QTY-EXP" sheetId="2" r:id="rId1"/>
     <sheet name="OPN" sheetId="1" r:id="rId2"/>
-    <sheet name="bacterial" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="20">
   <si>
     <t>OPN1MW</t>
   </si>
@@ -102,21 +101,6 @@
   <si>
     <t>HR
 trimer</t>
-  </si>
-  <si>
-    <t>QTY</t>
-  </si>
-  <si>
-    <t>WT</t>
-  </si>
-  <si>
-    <t>Monomer-trimer</t>
-  </si>
-  <si>
-    <t>HR</t>
-  </si>
-  <si>
-    <t>BR</t>
   </si>
 </sst>
 </file>
@@ -162,7 +146,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -185,37 +169,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="1" tint="0.499984740745262"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="1" tint="0.499984740745262"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1" tint="0.499984740745262"/>
-      </right>
-      <top style="thin">
-        <color theme="1" tint="0.499984740745262"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -233,19 +191,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -536,9 +482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D856C77-9565-4F87-ABAB-A87EC8DCE168}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D3"/>
-    </sheetView>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -563,13 +507,13 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>0.46800000000000003</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -577,13 +521,13 @@
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="8">
-        <v>0.60299999999999998</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="B3" s="7">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -591,13 +535,13 @@
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>0.48599999999999999</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -605,13 +549,13 @@
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="8">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="C5" s="8">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="D5" s="8">
+      <c r="B5" s="7">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="D5" s="7">
         <v>0.999</v>
       </c>
     </row>
@@ -619,13 +563,13 @@
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="8">
-        <v>0.45300000000000001</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="B6" s="7">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -633,13 +577,13 @@
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>0.307</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -647,13 +591,13 @@
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <v>0.55500000000000005</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -661,13 +605,13 @@
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="8">
-        <v>0.53100000000000003</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="8" t="s">
+      <c r="B9" s="7">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -675,13 +619,13 @@
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="8">
-        <v>0.55300000000000005</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="8" t="s">
+      <c r="B10" s="7">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -689,56 +633,56 @@
       <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="8">
-        <v>0.44700000000000001</v>
-      </c>
-      <c r="C11" s="8">
-        <v>0.45600000000000002</v>
-      </c>
-      <c r="D11" s="8">
-        <v>0.252</v>
+      <c r="B11" s="7">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.251</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0.45500000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="8">
-        <v>0.30599999999999999</v>
-      </c>
-      <c r="C12" s="8">
-        <v>0.34200000000000003</v>
-      </c>
-      <c r="D12" s="8">
-        <v>0.5</v>
+      <c r="B12" s="7">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.435</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="8">
-        <v>0.54100000000000004</v>
-      </c>
-      <c r="C13" s="8">
-        <v>0.21299999999999999</v>
-      </c>
-      <c r="D13" s="8">
-        <v>0.57099999999999995</v>
+      <c r="B13" s="7">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0.214</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0.54800000000000004</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="8">
-        <v>0.68899999999999995</v>
-      </c>
-      <c r="C14" s="8">
-        <v>0.28299999999999997</v>
-      </c>
-      <c r="D14" s="8">
-        <v>0.58399999999999996</v>
+      <c r="B14" s="7">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0.625</v>
       </c>
     </row>
   </sheetData>
@@ -750,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AC21" sqref="AC21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -815,50 +759,50 @@
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="13">
+      <c r="B2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="9">
         <v>0.17899999999999999</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="9">
         <v>0.84499999999999997</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="9">
         <v>0.91900000000000004</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="9">
         <v>1.6160000000000001</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="9">
         <v>1.0089999999999999</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="9">
         <v>1.2450000000000001</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="13">
+      <c r="K2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="9">
         <v>0.16900000000000001</v>
       </c>
-      <c r="M2" s="13">
+      <c r="M2" s="9">
         <v>0.76900000000000002</v>
       </c>
-      <c r="N2" s="13">
+      <c r="N2" s="9">
         <v>1.0449999999999999</v>
       </c>
-      <c r="O2" s="13">
+      <c r="O2" s="9">
         <v>1.613</v>
       </c>
-      <c r="P2" s="13">
+      <c r="P2" s="9">
         <v>1.1519999999999999</v>
       </c>
-      <c r="Q2" s="13">
+      <c r="Q2" s="9">
         <v>1.3720000000000001</v>
       </c>
     </row>
@@ -866,50 +810,50 @@
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="13">
+      <c r="B3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="9">
         <v>0.82299999999999995</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="9">
         <v>0.91300000000000003</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="9">
         <v>1.897</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="9">
         <v>0.92800000000000005</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="9">
         <v>1.5169999999999999</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="M3" s="13">
+      <c r="K3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="9">
         <v>0.77400000000000002</v>
       </c>
-      <c r="N3" s="13">
+      <c r="N3" s="9">
         <v>1.052</v>
       </c>
-      <c r="O3" s="13">
+      <c r="O3" s="9">
         <v>1.6539999999999999</v>
       </c>
-      <c r="P3" s="13">
+      <c r="P3" s="9">
         <v>1.155</v>
       </c>
-      <c r="Q3" s="13">
+      <c r="Q3" s="9">
         <v>1.141</v>
       </c>
     </row>
@@ -917,50 +861,50 @@
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="13">
+      <c r="B4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="9">
         <v>0.83399999999999996</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="9">
         <v>2.351</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="9">
         <v>1.101</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="9">
         <v>2.2949999999999999</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="N4" s="13">
+      <c r="K4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" s="9">
         <v>1.014</v>
       </c>
-      <c r="O4" s="13">
+      <c r="O4" s="9">
         <v>2.3159999999999998</v>
       </c>
-      <c r="P4" s="13">
+      <c r="P4" s="9">
         <v>1.1060000000000001</v>
       </c>
-      <c r="Q4" s="13">
+      <c r="Q4" s="9">
         <v>2.073</v>
       </c>
     </row>
@@ -968,50 +912,50 @@
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="13">
+      <c r="B5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="9">
         <v>2.2360000000000002</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="9">
         <v>1.0309999999999999</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="9">
         <v>1.8640000000000001</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="N5" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="O5" s="13">
+      <c r="K5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="9">
         <v>1.96</v>
       </c>
-      <c r="P5" s="13">
+      <c r="P5" s="9">
         <v>1.0169999999999999</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="Q5" s="9">
         <v>2.6829999999999998</v>
       </c>
     </row>
@@ -1019,50 +963,50 @@
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="13">
+      <c r="B6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="9">
         <v>1.0109999999999999</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="9">
         <v>1.155</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="M6" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="N6" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="O6" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="P6" s="13">
+      <c r="K6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="P6" s="9">
         <v>0.94499999999999995</v>
       </c>
-      <c r="Q6" s="13">
+      <c r="Q6" s="9">
         <v>1.194</v>
       </c>
     </row>
@@ -1070,50 +1014,50 @@
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="13">
+      <c r="B7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="9">
         <v>1.0109999999999999</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="N7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="O7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="P7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q7" s="13">
+      <c r="K7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="9">
         <v>1.1419999999999999</v>
       </c>
     </row>
@@ -1121,129 +1065,54 @@
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" s="12" t="s">
+      <c r="B8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>3</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="M8" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="N8" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="O8" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="P8" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q8" s="12" t="s">
+      <c r="K8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="8" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4911FA70-48E6-48E4-9139-2D9F96EC0E56}">
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="4" max="4" width="4.90625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="9"/>
-      <c r="E1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="9"/>
-    </row>
-    <row r="2" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
-      <c r="E2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="E3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="11"/>
-    </row>
-    <row r="4" spans="1:7" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add ChR2 superimposition figures. TODO: hydrophobicity surface
</commit_message>
<xml_diff>
--- a/QTY Design/Comparison.xlsx
+++ b/QTY Design/Comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\Rhodopsins_QTY\QTY Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9522EA8-C09A-4A44-8F76-6D933AD0EE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF95E94-144E-4A79-87EA-6EB9D33C66C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WT-QTY-EXP" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="48">
   <si>
     <t>OPN1MW</t>
   </si>
@@ -174,6 +174,20 @@
   </si>
   <si>
     <t>BACH QTY</t>
+  </si>
+  <si>
+    <t>ChR2</t>
+  </si>
+  <si>
+    <t>ChR2 QTY</t>
+  </si>
+  <si>
+    <t>CR
+dimer</t>
+  </si>
+  <si>
+    <t>CR
+monomer</t>
   </si>
 </sst>
 </file>
@@ -554,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D856C77-9565-4F87-ABAB-A87EC8DCE168}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -735,30 +749,58 @@
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B13" s="7">
-        <v>0.54400000000000004</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="C13" s="7">
-        <v>0.214</v>
+        <v>0.42699999999999999</v>
       </c>
       <c r="D13" s="7">
-        <v>0.54800000000000004</v>
+        <v>0.44700000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="7">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0.214</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0.54800000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B15" s="7">
         <v>0.68500000000000005</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C15" s="7">
         <v>0.20599999999999999</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D15" s="7">
         <v>0.625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="7">
+        <v>0.37</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0.51600000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -770,7 +812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="J2" sqref="J2:J8"/>
     </sheetView>
   </sheetViews>
@@ -1195,9 +1237,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE1B76D-EE64-4DB0-9876-AB8DCC598C18}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1587,6 +1629,37 @@
         <v>30.04</v>
       </c>
     </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="10">
+        <v>6.13</v>
+      </c>
+      <c r="D24" s="10">
+        <v>34.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="C25" s="10">
+        <v>6.13</v>
+      </c>
+      <c r="D25" s="10">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="E25">
+        <v>35.53</v>
+      </c>
+      <c r="F25">
+        <v>22.22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Switch to Overleaf TeX. Add RGR and RRH to all OPN superimposition
</commit_message>
<xml_diff>
--- a/QTY Design/Comparison.xlsx
+++ b/QTY Design/Comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\Rhodopsins_QTY\QTY Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF95E94-144E-4A79-87EA-6EB9D33C66C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0080CD-605C-4A7B-AA3B-66DCCB26988F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WT-QTY-EXP" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="48">
   <si>
     <t>OPN1MW</t>
   </si>
@@ -260,11 +260,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -576,230 +573,230 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="3"/>
+    <col min="1" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" s="4" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>0.46800000000000003</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="4" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>0.61099999999999999</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="C3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="4" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>0.48599999999999999</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="C4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="4" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>0.55900000000000005</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>0.54900000000000004</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>0.999</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:4" s="4" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>0.45400000000000001</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="C6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="4" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>0.307</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="C7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="4" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>0.55500000000000005</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="C8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="4" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>0.53700000000000003</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="C9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="4" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>0.54800000000000004</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+      <c r="C10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="4" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>0.44800000000000001</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>0.251</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>0.45500000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:4" s="4" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>0.29599999999999999</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>0.27400000000000002</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>0.435</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:4" s="4" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>0.23499999999999999</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>0.42699999999999999</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>0.44700000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:4" s="4" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>0.54400000000000004</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>0.214</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <v>0.54800000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:4" s="4" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>0.68500000000000005</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>0.20599999999999999</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>0.625</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="5" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:4" s="4" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>0.37</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>0.40899999999999997</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <v>0.51600000000000001</v>
       </c>
     </row>
@@ -810,423 +807,634 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="8" width="9.08984375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="4.54296875" customWidth="1"/>
+    <col min="1" max="10" width="9.08984375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:21" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="O1" s="4" t="s">
+      <c r="M1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="9">
+      <c r="T1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="8">
         <v>0.17899999999999999</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>0.84499999999999997</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>0.91900000000000004</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="8">
         <v>1.6160000000000001</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="8">
         <v>1.0089999999999999</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="8">
         <v>1.2450000000000001</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="9">
+      <c r="I2" s="8">
+        <v>1.131</v>
+      </c>
+      <c r="J2" s="8">
+        <v>1.7030000000000001</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="8">
         <v>0.16900000000000001</v>
       </c>
-      <c r="M2" s="9">
+      <c r="O2" s="8">
         <v>0.76900000000000002</v>
       </c>
-      <c r="N2" s="9">
+      <c r="P2" s="8">
         <v>1.0449999999999999</v>
       </c>
-      <c r="O2" s="9">
+      <c r="Q2" s="8">
         <v>1.613</v>
       </c>
-      <c r="P2" s="9">
+      <c r="R2" s="8">
         <v>1.1519999999999999</v>
       </c>
-      <c r="Q2" s="9">
+      <c r="S2" s="8">
         <v>1.3720000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="9">
+      <c r="T2" s="8">
+        <v>1.23</v>
+      </c>
+      <c r="U2" s="8">
+        <v>2.1779999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="8">
         <v>0.82299999999999995</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>0.91300000000000003</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <v>1.897</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="8">
         <v>0.92800000000000005</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="8">
         <v>1.5169999999999999</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="M3" s="9">
+      <c r="I3" s="8">
+        <v>1.1579999999999999</v>
+      </c>
+      <c r="J3" s="8">
+        <v>1.59</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" s="8">
         <v>0.77400000000000002</v>
       </c>
-      <c r="N3" s="9">
+      <c r="P3" s="8">
         <v>1.052</v>
       </c>
-      <c r="O3" s="9">
+      <c r="Q3" s="8">
         <v>1.6539999999999999</v>
       </c>
-      <c r="P3" s="9">
+      <c r="R3" s="8">
         <v>1.155</v>
       </c>
-      <c r="Q3" s="9">
+      <c r="S3" s="8">
         <v>1.141</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="9">
+      <c r="T3" s="8">
+        <v>1.3049999999999999</v>
+      </c>
+      <c r="U3" s="8">
+        <v>2.1930000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="8">
         <v>0.83399999999999996</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <v>2.351</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>1.101</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <v>2.2949999999999999</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="N4" s="9">
+      <c r="I4" s="8">
+        <v>1.0449999999999999</v>
+      </c>
+      <c r="J4" s="8">
+        <v>2.7029999999999998</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" s="8">
         <v>1.014</v>
       </c>
-      <c r="O4" s="9">
+      <c r="Q4" s="8">
         <v>2.3159999999999998</v>
       </c>
-      <c r="P4" s="9">
+      <c r="R4" s="8">
         <v>1.1060000000000001</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="S4" s="8">
         <v>2.073</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="9">
+      <c r="T4" s="8">
+        <v>1.173</v>
+      </c>
+      <c r="U4" s="8">
+        <v>1.9419999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="8">
         <v>2.2360000000000002</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>1.0309999999999999</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <v>1.8640000000000001</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="O5" s="9">
+      <c r="I5" s="8">
+        <v>1.369</v>
+      </c>
+      <c r="J5" s="8">
+        <v>2.0979999999999999</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="8">
         <v>1.96</v>
       </c>
-      <c r="P5" s="9">
+      <c r="R5" s="8">
         <v>1.0169999999999999</v>
       </c>
-      <c r="Q5" s="9">
+      <c r="S5" s="8">
         <v>2.6829999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="T5" s="8">
+        <v>1.397</v>
+      </c>
+      <c r="U5" s="8">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="9">
+      <c r="B6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="8">
         <v>1.0109999999999999</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="8">
         <v>1.155</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="4" t="s">
+      <c r="I6" s="8">
+        <v>1.671</v>
+      </c>
+      <c r="J6" s="8">
+        <v>1.343</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="O6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="P6" s="9">
+      <c r="M6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="R6" s="8">
         <v>0.94499999999999995</v>
       </c>
-      <c r="Q6" s="9">
+      <c r="S6" s="8">
         <v>1.194</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="T6" s="8">
+        <v>1.512</v>
+      </c>
+      <c r="U6" s="8">
+        <v>1.077</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="9">
+      <c r="B7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="8">
         <v>1.0109999999999999</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="4" t="s">
+      <c r="I7" s="7">
+        <v>1.3580000000000001</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="L7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="O7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="P7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q7" s="9">
+      <c r="M7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="S7" s="8">
         <v>1.1419999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+      <c r="T7" s="7">
+        <v>1.264</v>
+      </c>
+      <c r="U7" s="8">
+        <v>1.0349999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="4" t="s">
+      <c r="B8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="7">
+        <v>1.5309999999999999</v>
+      </c>
+      <c r="J8" s="7">
+        <v>1.353</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="O8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="P8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q8" s="8" t="s">
+      <c r="M8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="R8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="S8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="T8" s="7">
+        <v>1.478</v>
+      </c>
+      <c r="U8" s="7">
+        <v>1.175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="8">
+        <v>1.3120000000000001</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="R9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="T9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="U9" s="8">
+        <v>1.079</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="R10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="S10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="T10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="U10" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1239,7 +1447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE1B76D-EE64-4DB0-9876-AB8DCC598C18}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1270,14 +1478,14 @@
       <c r="A2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="9">
         <v>8.9</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="9">
         <v>40.58</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -1286,16 +1494,16 @@
       <c r="B3">
         <v>0.46800000000000003</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>8.82</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>40.85</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>41.86</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="9">
         <v>19.78</v>
       </c>
     </row>
@@ -1303,14 +1511,14 @@
       <c r="A4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>8.89</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>40.57</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -1319,16 +1527,16 @@
       <c r="B5">
         <v>0.61099999999999999</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>8.83</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>40.76</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>40.119999999999997</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>18.96</v>
       </c>
     </row>
@@ -1336,14 +1544,14 @@
       <c r="A6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>8.75</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>38.72</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -1352,16 +1560,16 @@
       <c r="B7">
         <v>0.48599999999999999</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>8.66</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>39.299999999999997</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>46.51</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
         <v>23.19</v>
       </c>
     </row>
@@ -1369,14 +1577,14 @@
       <c r="A8" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>6.2</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>38.89</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -1385,16 +1593,16 @@
       <c r="B9">
         <v>0.55900000000000005</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>6.2</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>39.29</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>46.58</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="9">
         <v>21.55</v>
       </c>
     </row>
@@ -1402,14 +1610,14 @@
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>9.2899999999999991</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>44.87</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -1418,16 +1626,16 @@
       <c r="B11">
         <v>0.45400000000000001</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <v>9.18</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>45.47</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>49.12</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <v>20.9</v>
       </c>
     </row>
@@ -1435,14 +1643,14 @@
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <v>9.35</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <v>52.64</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1451,16 +1659,16 @@
       <c r="B13">
         <v>0.307</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <v>9.19</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>53.08</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="9">
         <v>50.34</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="9">
         <v>15.48</v>
       </c>
     </row>
@@ -1468,14 +1676,14 @@
       <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <v>9.11</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <v>39.729999999999997</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -1484,16 +1692,16 @@
       <c r="B15">
         <v>0.55500000000000005</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="9">
         <v>9.02</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <v>40.04</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="9">
         <v>45.58</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="9">
         <v>18.93</v>
       </c>
     </row>
@@ -1501,14 +1709,14 @@
       <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="9">
         <v>8.34</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="9">
         <v>31.87</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
@@ -1517,16 +1725,16 @@
       <c r="B17">
         <v>0.53700000000000003</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="9">
         <v>8.2899999999999991</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="9">
         <v>32.39</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="9">
         <v>42.86</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="9">
         <v>21.65</v>
       </c>
     </row>
@@ -1534,14 +1742,14 @@
       <c r="A18" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="9">
         <v>8.77</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="9">
         <v>37.42</v>
       </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -1550,16 +1758,16 @@
       <c r="B19">
         <v>0.54800000000000004</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="9">
         <v>8.7200000000000006</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="9">
         <v>37.46</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="9">
         <v>40.96</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="9">
         <v>20.18</v>
       </c>
     </row>
@@ -1567,14 +1775,14 @@
       <c r="A20" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="9">
         <v>4.75</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="9">
         <v>26.92</v>
       </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
@@ -1583,16 +1791,16 @@
       <c r="B21">
         <v>0.44800000000000001</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="9">
         <v>4.75</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="9">
         <v>27.4</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="9">
         <v>46.67</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="9">
         <v>25.3</v>
       </c>
     </row>
@@ -1600,14 +1808,14 @@
       <c r="A22" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="9">
         <v>5.34</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="9">
         <v>26.96</v>
       </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -1616,16 +1824,16 @@
       <c r="B23">
         <v>0.29599999999999999</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="9">
         <v>5.34</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="9">
         <v>27.5</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="9">
         <v>44.19</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="9">
         <v>30.04</v>
       </c>
     </row>
@@ -1633,10 +1841,10 @@
       <c r="A24" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="9">
         <v>6.13</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="9">
         <v>34.9</v>
       </c>
     </row>
@@ -1647,10 +1855,10 @@
       <c r="B25">
         <v>0.23499999999999999</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="9">
         <v>6.13</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="9">
         <v>35.299999999999997</v>
       </c>
       <c r="E25">

</xml_diff>

<commit_message>
Write results and discussion
</commit_message>
<xml_diff>
--- a/QTY Design/Comparison.xlsx
+++ b/QTY Design/Comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\Rhodopsins_QTY\QTY Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0080CD-605C-4A7B-AA3B-66DCCB26988F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704CDEFC-0A3A-49A0-B005-E91B7FC341E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WT-QTY-EXP" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="49">
   <si>
     <t>OPN1MW</t>
   </si>
@@ -188,6 +188,9 @@
   <si>
     <t>CR
 monomer</t>
+  </si>
+  <si>
+    <t>DIFF</t>
   </si>
 </sst>
 </file>
@@ -807,18 +810,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:AF10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AH18" sqref="AH18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="10" width="9.08984375" style="2" customWidth="1"/>
+    <col min="25" max="25" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -879,8 +883,38 @@
       <c r="U1" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="W1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -941,8 +975,46 @@
       <c r="U2" s="8">
         <v>2.1779999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="W2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="8">
+        <f>N2-C2</f>
+        <v>-9.9999999999999811E-3</v>
+      </c>
+      <c r="Z2" s="8">
+        <f t="shared" ref="Z2:AF9" si="0">O2-D2</f>
+        <v>-7.5999999999999956E-2</v>
+      </c>
+      <c r="AA2" s="8">
+        <f t="shared" si="0"/>
+        <v>0.12599999999999989</v>
+      </c>
+      <c r="AB2" s="8">
+        <f t="shared" si="0"/>
+        <v>-3.0000000000001137E-3</v>
+      </c>
+      <c r="AC2" s="8">
+        <f t="shared" si="0"/>
+        <v>0.14300000000000002</v>
+      </c>
+      <c r="AD2" s="8">
+        <f t="shared" si="0"/>
+        <v>0.127</v>
+      </c>
+      <c r="AE2" s="8">
+        <f t="shared" si="0"/>
+        <v>9.8999999999999977E-2</v>
+      </c>
+      <c r="AF2" s="8">
+        <f t="shared" si="0"/>
+        <v>0.47499999999999987</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1003,8 +1075,45 @@
       <c r="U3" s="8">
         <v>2.1930000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="W3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z3" s="8">
+        <f t="shared" si="0"/>
+        <v>-4.8999999999999932E-2</v>
+      </c>
+      <c r="AA3" s="8">
+        <f t="shared" si="0"/>
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="AB3" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.2430000000000001</v>
+      </c>
+      <c r="AC3" s="8">
+        <f t="shared" si="0"/>
+        <v>0.22699999999999998</v>
+      </c>
+      <c r="AD3" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.37599999999999989</v>
+      </c>
+      <c r="AE3" s="8">
+        <f t="shared" si="0"/>
+        <v>0.14700000000000002</v>
+      </c>
+      <c r="AF3" s="8">
+        <f t="shared" si="0"/>
+        <v>0.60299999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1065,8 +1174,44 @@
       <c r="U4" s="8">
         <v>1.9419999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="W4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA4" s="8">
+        <f t="shared" si="0"/>
+        <v>0.18000000000000005</v>
+      </c>
+      <c r="AB4" s="8">
+        <f t="shared" si="0"/>
+        <v>-3.5000000000000142E-2</v>
+      </c>
+      <c r="AC4" s="8">
+        <f t="shared" si="0"/>
+        <v>5.0000000000001155E-3</v>
+      </c>
+      <c r="AD4" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.22199999999999998</v>
+      </c>
+      <c r="AE4" s="8">
+        <f t="shared" si="0"/>
+        <v>0.12800000000000011</v>
+      </c>
+      <c r="AF4" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.7609999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1127,8 +1272,43 @@
       <c r="U5" s="8">
         <v>1.01</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="W5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB5" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.27600000000000025</v>
+      </c>
+      <c r="AC5" s="8">
+        <f t="shared" si="0"/>
+        <v>-1.4000000000000012E-2</v>
+      </c>
+      <c r="AD5" s="8">
+        <f t="shared" si="0"/>
+        <v>0.81899999999999973</v>
+      </c>
+      <c r="AE5" s="8">
+        <f t="shared" si="0"/>
+        <v>2.8000000000000025E-2</v>
+      </c>
+      <c r="AF5" s="8">
+        <f t="shared" si="0"/>
+        <v>-1.0879999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1189,8 +1369,42 @@
       <c r="U6" s="8">
         <v>1.077</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="W6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC6" s="8">
+        <f t="shared" si="0"/>
+        <v>-6.5999999999999948E-2</v>
+      </c>
+      <c r="AD6" s="8">
+        <f t="shared" si="0"/>
+        <v>3.8999999999999924E-2</v>
+      </c>
+      <c r="AE6" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.15900000000000003</v>
+      </c>
+      <c r="AF6" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.26600000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -1251,8 +1465,41 @@
       <c r="U7" s="8">
         <v>1.0349999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="W7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="AE7" s="8">
+        <f t="shared" si="0"/>
+        <v>-9.4000000000000083E-2</v>
+      </c>
+      <c r="AF7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.11799999999999988</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1313,8 +1560,40 @@
       <c r="U8" s="7">
         <v>1.175</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="W8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE8" s="8">
+        <f t="shared" si="0"/>
+        <v>-5.2999999999999936E-2</v>
+      </c>
+      <c r="AF8" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.17799999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -1375,8 +1654,39 @@
       <c r="U9" s="8">
         <v>1.079</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="W9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="X9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF9" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.2330000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1435,6 +1745,36 @@
         <v>3</v>
       </c>
       <c r="U10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="X10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF10" s="7" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>